<commit_message>
Adiciona tela de dashboard estática
</commit_message>
<xml_diff>
--- a/Documentos/Backlogs/Sprint-Backlog1.xlsx
+++ b/Documentos/Backlogs/Sprint-Backlog1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/vinicius_n_ferreira_accenture_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/vinicius_n_ferreira_accenture_com/Documents/Desktop/Grupo07-Backup/Documentos/Backlogs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="8_{B8FCD2F3-E2C3-4CE9-9340-BB5A1D9322D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D3045485-5A00-422E-BDC9-4E58646B72A2}"/>
+  <xr:revisionPtr revIDLastSave="308" documentId="8_{B8FCD2F3-E2C3-4CE9-9340-BB5A1D9322D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1A6E3E52-C598-4554-A214-2510228906B0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{4463D4C9-A9DF-4424-8611-E309CA78F67D}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_Requisitos!$B$2:$K$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Lista_Requisitos_Sprint1!$B$2:$I$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Lista_Requisitos_Sprint1!$B$2:$I$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>Essencial</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Luiz Gustavo</t>
   </si>
   <si>
-    <t>Foi desenvolvido duas proto-personas referentes ao dois usuários da plataforma (desenvolvedor e investidor)</t>
-  </si>
-  <si>
     <t>Desenvolvido o mapa de empatia referente ao nosso principal usuário da plataforma (desenvolvedor)</t>
   </si>
   <si>
@@ -215,6 +212,12 @@
   </si>
   <si>
     <t>Escolha de uma ferramenta de gestão para controlar o que é desenvolvido durante as reuniões (Atas)</t>
+  </si>
+  <si>
+    <t>Foi desenvolvido a proto-personas referente a o desenvolvedor.</t>
+  </si>
+  <si>
+    <t>Foi desenvolvido a proto-personas referente a o investidor.</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1269,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
@@ -1333,7 +1336,7 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="24"/>
       <c r="B3" s="30">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>34</v>
@@ -1358,7 +1361,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="24"/>
       <c r="B4" s="30">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>42</v>
@@ -1385,7 +1388,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="24"/>
       <c r="B5" s="30">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>43</v>
@@ -1412,7 +1415,7 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="30">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>44</v>
@@ -1439,10 +1442,10 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="30">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="31">
         <v>44416</v>
@@ -1455,7 +1458,7 @@
         <v>48</v>
       </c>
       <c r="H7" s="34">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="25"/>
@@ -1464,10 +1467,10 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="30">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="31">
         <v>44416</v>
@@ -1489,7 +1492,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="30">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>46</v>
@@ -1514,7 +1517,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="30">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>45</v>
@@ -1539,7 +1542,7 @@
     <row r="11" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="30">
-        <v>14</v>
+        <v>14.1</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>47</v>
@@ -1555,7 +1558,7 @@
         <v>48</v>
       </c>
       <c r="H11" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="24"/>
@@ -1564,10 +1567,10 @@
     <row r="12" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="30">
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="31">
         <v>44434</v>
@@ -1580,7 +1583,7 @@
         <v>49</v>
       </c>
       <c r="H12" s="9">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="27"/>
@@ -1589,10 +1592,10 @@
     <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="30">
-        <v>14.2</v>
+        <v>14.3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D13" s="31">
         <v>44427</v>
@@ -1611,120 +1614,132 @@
       <c r="J13" s="24"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="30">
-        <v>14.3</v>
+        <v>14.4</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D14" s="31">
         <v>44427</v>
       </c>
       <c r="E14" s="31">
-        <v>44446</v>
+        <v>44434</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H14" s="9">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I14" s="20"/>
-      <c r="J14" s="27"/>
+      <c r="J14" s="24"/>
       <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="30">
-        <v>14.4</v>
+        <v>14.5</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" s="31">
-        <v>44440</v>
+        <v>44427</v>
       </c>
       <c r="E15" s="31">
         <v>44446</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H15" s="9">
         <v>14</v>
       </c>
       <c r="I15" s="20"/>
-      <c r="J15" s="24"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="30">
-        <v>14.5</v>
+        <v>14.6</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D16" s="31">
-        <v>44434</v>
+        <v>44440</v>
       </c>
       <c r="E16" s="31">
-        <v>44440</v>
+        <v>44446</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H16" s="9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="24"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
       <c r="B17" s="30">
-        <v>14.6</v>
+        <v>14.7</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="31">
-        <v>44427</v>
+        <v>44434</v>
       </c>
       <c r="E17" s="31">
         <v>44440</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H17" s="9">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I17" s="20"/>
       <c r="J17" s="24"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="19"/>
+      <c r="B18" s="30">
+        <v>14.8</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="31">
+        <v>44427</v>
+      </c>
+      <c r="E18" s="31">
+        <v>44440</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="9">
+        <v>4</v>
+      </c>
+      <c r="I18" s="20"/>
       <c r="J18" s="24"/>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="24"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
@@ -1737,7 +1752,7 @@
       <c r="J19" s="24"/>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
@@ -1750,7 +1765,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
@@ -1763,7 +1778,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="11"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
@@ -1776,7 +1791,7 @@
       <c r="J22" s="24"/>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
@@ -1789,7 +1804,7 @@
       <c r="J23" s="24"/>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
@@ -1802,7 +1817,7 @@
       <c r="J24" s="24"/>
       <c r="K24" s="11"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
@@ -1815,31 +1830,33 @@
       <c r="J25" s="24"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="11"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="19"/>
       <c r="J26" s="24"/>
       <c r="K26" s="11"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="24"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="41"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="11"/>
       <c r="J27" s="24"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="29"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
@@ -1850,7 +1867,7 @@
       <c r="H28" s="41"/>
       <c r="J28" s="24"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="29"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
@@ -1861,7 +1878,7 @@
       <c r="H29" s="41"/>
       <c r="J29" s="24"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="29"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
@@ -1872,7 +1889,7 @@
       <c r="H30" s="41"/>
       <c r="J30" s="24"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="29"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
@@ -1883,22 +1900,19 @@
       <c r="H31" s="41"/>
       <c r="J31" s="24"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="29"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="41"/>
       <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="24"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
       <c r="D33" s="32"/>
@@ -1911,6 +1925,20 @@
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
     </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" scale="74" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>